<commit_message>
update hangboard entries as well as error check to account for any erros in the one-handed entries
</commit_message>
<xml_diff>
--- a/TrevorHB_kg.xlsx
+++ b/TrevorHB_kg.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="171">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -130,7 +130,7 @@
     <t xml:space="preserve">-9,3,7,7,6</t>
   </si>
   <si>
-    <t xml:space="preserve">-20,0</t>
+    <t xml:space="preserve">-20,0,1,1,1,1,1,1</t>
   </si>
   <si>
     <t xml:space="preserve">-18.5,6</t>
@@ -229,7 +229,7 @@
     <t xml:space="preserve">-14.5,4,9,7</t>
   </si>
   <si>
-    <t xml:space="preserve">-9,5,8,8</t>
+    <t xml:space="preserve">-9,4,8,8</t>
   </si>
   <si>
     <t xml:space="preserve">-17,6</t>
@@ -250,7 +250,7 @@
     <t xml:space="preserve">-9,3,7,6,5</t>
   </si>
   <si>
-    <t xml:space="preserve">R,14,6:L,14,2,6,4,4,4</t>
+    <t xml:space="preserve">R,14,6:L,14,2,7,5,6,5</t>
   </si>
   <si>
     <t xml:space="preserve">-16,5,7</t>
@@ -271,7 +271,7 @@
     <t xml:space="preserve">-8.5,3,6,6,7</t>
   </si>
   <si>
-    <t xml:space="preserve">R,14,6:L,14,4,6,6,8</t>
+    <t xml:space="preserve">R,14,6:L,14,3,6,6,8</t>
   </si>
   <si>
     <t xml:space="preserve">-6,5,9</t>
@@ -322,7 +322,7 @@
     <t xml:space="preserve">-8,4,8,5</t>
   </si>
   <si>
-    <t xml:space="preserve">R,15,6:L,15,2.5,7,5,5</t>
+    <t xml:space="preserve">R,15,6:L,15,2,5,7,5,5</t>
   </si>
   <si>
     <t xml:space="preserve">-13.5,5,8</t>
@@ -338,6 +338,201 @@
   </si>
   <si>
     <t xml:space="preserve">-13.5,5,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Mar 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-8.5,4,7,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L,14,6:R,14,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L,12,5,5:R,12,5,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Mar 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-8.5,5,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L,14.5,3,7,8,4:R,14.5,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L,12.5,4,7,5:R,12.5,5,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 Mar 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-3.5,4,9,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-8.5,3,5,8,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L,14.5,6:R,14.5,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L,12.5,4,7,4:R,12.5,4,4,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-16.5,5,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 Mar 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-3.5,5,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-8.5,5,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L,14.5,3,8,5,6:R,14.5,5,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-4,5,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L,12.5,2,5,5,5,4:R,12.5,4,8,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22 Mar 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-3.5,5,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-8.5,3,8,6,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R,14.5,5,9:L,14.5,4,6,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-13,5,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-4,3,8,8,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R,12.5,4,6,6:L,12.5,3,7,6,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-16,3,9,8,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-13.5,4,6,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 Apr 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-3.5,4,8,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R,14.5,6:L,14.5,4,8,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-12.5,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R,12.5,5,9:L,12.5,2,7,7,7,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-16,4,8,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 Apr 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-3.5,5,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-8,3,7,6,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R,15,6:L,15,4,7,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R,13,4,6,6:L,13,4,9,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-16,3,8,8,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-13,4,4,8,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 May 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-3.5,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-8,4,6,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R,15,6:L,15,3,8,5,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-11.5,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R,13,3,9,7,7:L,13,2,8,6,5,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-16,3,7,7,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-13,5,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 Jul 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-8.5,5,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L,14.5,2,4,7,6,6:R,14.5,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-13,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L,12.5,2,6,6,3,3:R,12.5,4,5,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-16,4,7,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-13.5,5,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19 Jul 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-3,4,9,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-8,4,5,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R,15,6:L,14.5,5,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-12.5,5,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R,12.5,3,9,6,7:L,12.5,3,6,5,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-16,2,8,7,7,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-13,3,6,8,7</t>
   </si>
 </sst>
 </file>
@@ -443,16 +638,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
+      <selection pane="topLeft" activeCell="H28" activeCellId="0" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="21.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1032,98 +1227,324 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
+      <c r="A19" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
+      <c r="A20" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
+      <c r="A21" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
+      <c r="A22" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
+      <c r="A23" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
+      <c r="A24" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
+      <c r="A25" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
+      <c r="A26" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>170</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>